<commit_message>
ubah detail export excel (+ketidakhadiran)
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>No.</t>
   </si>
@@ -36,13 +36,22 @@
   </si>
   <si>
     <t>Alamat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>JEMAAT YANG HADIR</t>
+  </si>
+  <si>
+    <t>JEMAAT YANG TIDAK HADIR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +62,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -94,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -133,6 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,45 +442,69 @@
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="79.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>